<commit_message>
Revert "Merge branch 'dev' of https://github.com/imagilex/simma-facturacion into SMF045"
This reverts commit 90f8878637b25f84143ec796bdf8bb2ab79fe92d.
</commit_message>
<xml_diff>
--- a/project_files/files/templates/clientes.xlsx
+++ b/project_files/files/templates/clientes.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\simma-facturacion\project_files\files\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="761"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="GENERADORES" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GENERADORES!$A$1:$BD$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GENERADORES!$A$1:$BC$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -31,10 +26,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>RRamirez</author>
-    <author>FROSTBITEinternex</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -130,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -226,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -250,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -274,32 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -347,7 +316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -371,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -392,266 +361,6 @@
           </rPr>
           <t xml:space="preserve">
 El valor debe corresponder con el catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BG1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">CarlosGutiérrez:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BH1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BI1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BJ1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BK1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BL1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BM1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BO1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BP1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BQ1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
         </r>
       </text>
     </comment>
@@ -663,10 +372,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>RRamirez</author>
-    <author>FROSTBITEinternex</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -690,7 +398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -714,7 +422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -738,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -762,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -786,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -810,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -834,7 +542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -858,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -882,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -906,7 +614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -930,7 +638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -954,7 +662,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -978,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1002,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1026,32 +734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>CarlosGutiérrez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-El valor debe corresponder con el
-catalogo del sistema</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AN1" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1075,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0" shapeId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1104,7 +787,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
   <si>
     <t>No.</t>
   </si>
@@ -1290,67 +973,13 @@
   </si>
   <si>
     <t>Nombre Corto</t>
-  </si>
-  <si>
-    <t>Categoria del cliente</t>
-  </si>
-  <si>
-    <t>Moneda</t>
-  </si>
-  <si>
-    <t>Uso del CFDI</t>
-  </si>
-  <si>
-    <t>Clave del Producto o Servicio</t>
-  </si>
-  <si>
-    <t>Clave de Unidad</t>
-  </si>
-  <si>
-    <t>Unidad</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>Impuesto</t>
-  </si>
-  <si>
-    <t>Tipo de Factor</t>
-  </si>
-  <si>
-    <t>Tasa O Cuota</t>
-  </si>
-  <si>
-    <t>Cuenta</t>
-  </si>
-  <si>
-    <t>CLABE</t>
-  </si>
-  <si>
-    <t>RFC del Banco</t>
-  </si>
-  <si>
-    <t>Banco</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
-    <t>Forma de Pago</t>
-  </si>
-  <si>
-    <t>Método de Pago CFDI</t>
-  </si>
-  <si>
-    <t>Unidad de Facturación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1392,32 +1021,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1445,10 +1048,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,7 +1351,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1757,13 +1359,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="BT11" sqref="BT11"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC1" sqref="BC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1799,45 +1401,32 @@
     <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="21" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.85546875" customWidth="1"/>
-    <col min="36" max="36" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="27.7109375" customWidth="1"/>
-    <col min="60" max="61" width="19.85546875" customWidth="1"/>
-    <col min="62" max="62" width="28.85546875" customWidth="1"/>
-    <col min="63" max="63" width="17.42578125" customWidth="1"/>
-    <col min="64" max="64" width="38.28515625" customWidth="1"/>
-    <col min="65" max="65" width="21.85546875" customWidth="1"/>
-    <col min="67" max="67" width="13.42578125" customWidth="1"/>
-    <col min="68" max="68" width="19" customWidth="1"/>
-    <col min="69" max="69" width="18.42578125" customWidth="1"/>
-    <col min="70" max="70" width="17.28515625" customWidth="1"/>
-    <col min="72" max="72" width="19.28515625" customWidth="1"/>
-    <col min="73" max="73" width="18.7109375" customWidth="1"/>
+    <col min="35" max="35" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="22" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1941,127 +1530,73 @@
         <v>27</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BF1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BM1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BR1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2073,13 +1608,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE1"/>
+  <dimension ref="A1:BD1"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM3" sqref="AM3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -2119,28 +1652,27 @@
     <col min="36" max="36" width="9" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="21" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="29.140625" customWidth="1"/>
-    <col min="40" max="40" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:56" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -2256,60 +1788,57 @@
         <v>27</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BE1" s="1" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>